<commit_message>
Loading the data and searching the items on google. Adding selenium WebDriver
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani Debastiani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani Debastiani\Desktop\Automação - Busca por imagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70DC9480-98B9-40C4-83D3-1F0E989B43E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9C2EB7-3E5E-45CD-8D07-12300D33AA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5CAD714F-BE44-4496-980E-1AE735E7C190}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>

<commit_message>
inserting as images into the spreadsheet
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -1,100 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani Debastiani\Desktop\Automação - Busca por imagens\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A407F955-70EA-4881-8C1C-5186C92B021C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5CAD714F-BE44-4496-980E-1AE735E7C190}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Produtos" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
-  <si>
-    <t>Produto</t>
-  </si>
-  <si>
-    <t>Cor</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Xiaomi</t>
-  </si>
-  <si>
-    <t>Note 7</t>
-  </si>
-  <si>
-    <t>Branco</t>
-  </si>
-  <si>
-    <t>Preto</t>
-  </si>
-  <si>
-    <t>Note 10</t>
-  </si>
-  <si>
-    <t>Verde</t>
-  </si>
-  <si>
-    <t>Imagem</t>
-  </si>
-  <si>
-    <t>Karsten</t>
-  </si>
-  <si>
-    <t>Toalha de Rosto Lumina</t>
-  </si>
-  <si>
-    <t>Trussardi</t>
-  </si>
-  <si>
-    <t>Azul</t>
-  </si>
-  <si>
-    <t>Toalha de Rosto Imperiale</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -113,22 +46,307 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1409700" cy="1838325"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1714500" cy="1714500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1381125" cy="1771650"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1009650" cy="2047875"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>5</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1714500" cy="1714500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>6</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1714500" cy="1714500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1181100" cy="2047875"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>8</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1809750" cy="1809750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,96 +645,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA1EAC1-57EA-49E4-A8C1-10E0B14F1C6D}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="26.5703125" defaultRowHeight="142.5" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
+    <row r="1" ht="142.5" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Marca</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Produto</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cor</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Imagem</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    <row r="2" ht="142.5" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Note 7</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Branco</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+    <row r="3" ht="142.5" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Note 7</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Preto</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+    <row r="4" ht="142.5" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Note 10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Verde</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+    <row r="5" ht="142.5" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Note 10</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Branco</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
+    <row r="6" ht="142.5" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Karsten</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Toalha de Rosto Lumina</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Preto</t>
+        </is>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
+    <row r="7" ht="140.25" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Trussardi</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Toalha de Rosto Imperiale</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Verde</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="142.5" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dolce Gusto</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mine Me</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="142.5" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Nespresso</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Inissinia D40</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Vermelha</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>